<commit_message>
Revised functions. Changed example data to Station ALOHA. Finalized assessment model runs. Updated assessment diagnostics.
</commit_message>
<xml_diff>
--- a/Data/AA-CSIA_ALOHA_Summer.xlsx
+++ b/Data/AA-CSIA_ALOHA_Summer.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28324"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40c9661624813381/Documents/R/Tracing-Organic-Matter-in-Planktonic-Foodwebs-Using-Bayesian-Analysis/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/40c9661624813381/Documents/R/AA-CSIA-Organic-Matter-Supply-Model/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="943" documentId="13_ncr:1_{47D0C447-CF42-44CE-A2DC-F04BD3ED6669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1A7E0069-168A-4766-ADF7-097FDDB17CE4}"/>
+  <xr:revisionPtr revIDLastSave="952" documentId="13_ncr:1_{47D0C447-CF42-44CE-A2DC-F04BD3ED6669}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{95C97456-2786-4E8E-80D5-C564271E1E04}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-13395" windowWidth="29040" windowHeight="17520" firstSheet="1" activeTab="1" xr2:uid="{8FC557E2-921B-4618-B5F4-A9A2FDF78F4B}"/>
+    <workbookView xWindow="-90" yWindow="-90" windowWidth="19380" windowHeight="11460" firstSheet="1" activeTab="1" xr2:uid="{8FC557E2-921B-4618-B5F4-A9A2FDF78F4B}"/>
   </bookViews>
   <sheets>
     <sheet name="Zooplankton Biomass Data" sheetId="1" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1355" uniqueCount="136">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="136">
   <si>
     <t>Tow</t>
   </si>
@@ -326,9 +326,6 @@
     <t>Pump Cast</t>
   </si>
   <si>
-    <t>unk</t>
-  </si>
-  <si>
     <t>Supor</t>
   </si>
   <si>
@@ -450,6 +447,9 @@
   </si>
   <si>
     <t>SDd15NLys</t>
+  </si>
+  <si>
+    <t>Taxa</t>
   </si>
 </sst>
 </file>
@@ -748,6 +748,10 @@
     <xdr:clientData/>
   </xdr:oneCellAnchor>
 </xdr:wsDr>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -22716,10 +22720,10 @@
   <dimension ref="A1:AN94"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <pane xSplit="12" ySplit="1" topLeftCell="M2" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="12" ySplit="1" topLeftCell="M42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="J1" sqref="J1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="AA3" sqref="AA3"/>
+      <selection pane="bottomRight" activeCell="I65" sqref="I65"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.75" x14ac:dyDescent="0.75"/>
@@ -22740,7 +22744,7 @@
   <sheetData>
     <row r="1" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A1" s="1" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>35</v>
@@ -22764,7 +22768,7 @@
         <v>7</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="J1" s="1" t="s">
         <v>79</v>
@@ -22776,93 +22780,93 @@
         <v>30</v>
       </c>
       <c r="M1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="N1" s="3" t="s">
         <v>108</v>
       </c>
-      <c r="N1" s="3" t="s">
+      <c r="O1" s="4" t="s">
         <v>109</v>
       </c>
-      <c r="O1" s="4" t="s">
+      <c r="P1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="P1" s="3" t="s">
+      <c r="Q1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="Q1" s="4" t="s">
+      <c r="R1" s="4" t="s">
         <v>112</v>
       </c>
-      <c r="R1" s="4" t="s">
+      <c r="S1" s="4" t="s">
         <v>113</v>
       </c>
-      <c r="S1" s="4" t="s">
+      <c r="T1" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="T1" s="3" t="s">
+      <c r="U1" s="3" t="s">
         <v>115</v>
       </c>
-      <c r="U1" s="3" t="s">
+      <c r="V1" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="V1" s="5" t="s">
+      <c r="W1" s="3" t="s">
         <v>117</v>
       </c>
-      <c r="W1" s="3" t="s">
+      <c r="X1" s="4" t="s">
         <v>118</v>
       </c>
-      <c r="X1" s="4" t="s">
+      <c r="Y1" s="3" t="s">
         <v>119</v>
       </c>
-      <c r="Y1" s="3" t="s">
+      <c r="Z1" s="4" t="s">
         <v>120</v>
       </c>
-      <c r="Z1" s="4" t="s">
+      <c r="AA1" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="AA1" s="3" t="s">
+      <c r="AB1" s="3" t="s">
         <v>122</v>
       </c>
-      <c r="AB1" s="3" t="s">
+      <c r="AC1" s="4" t="s">
         <v>123</v>
       </c>
-      <c r="AC1" s="4" t="s">
+      <c r="AD1" s="3" t="s">
         <v>124</v>
       </c>
-      <c r="AD1" s="3" t="s">
+      <c r="AE1" s="4" t="s">
         <v>125</v>
       </c>
-      <c r="AE1" s="4" t="s">
+      <c r="AF1" s="4" t="s">
         <v>126</v>
       </c>
-      <c r="AF1" s="4" t="s">
+      <c r="AG1" s="4" t="s">
         <v>127</v>
       </c>
-      <c r="AG1" s="4" t="s">
+      <c r="AH1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="AH1" s="3" t="s">
+      <c r="AI1" s="3" t="s">
         <v>129</v>
       </c>
-      <c r="AI1" s="3" t="s">
+      <c r="AJ1" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="AJ1" s="5" t="s">
+      <c r="AK1" s="3" t="s">
         <v>131</v>
       </c>
-      <c r="AK1" s="3" t="s">
+      <c r="AL1" s="4" t="s">
         <v>132</v>
       </c>
-      <c r="AL1" s="4" t="s">
+      <c r="AM1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="AM1" s="3" t="s">
+      <c r="AN1" s="4" t="s">
         <v>134</v>
-      </c>
-      <c r="AN1" s="4" t="s">
-        <v>135</v>
       </c>
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A2" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>92</v>
@@ -22874,10 +22878,10 @@
         <v>25</v>
       </c>
       <c r="G2" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H2" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I2" t="s">
         <v>76</v>
@@ -22886,7 +22890,7 @@
         <v>81</v>
       </c>
       <c r="K2" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M2" s="12">
         <v>2.5062000000000002</v>
@@ -22971,7 +22975,7 @@
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>92</v>
@@ -22983,10 +22987,10 @@
         <v>150</v>
       </c>
       <c r="G3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H3" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I3" t="s">
         <v>76</v>
@@ -23084,7 +23088,7 @@
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A4" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>92</v>
@@ -23096,10 +23100,10 @@
         <v>247.5</v>
       </c>
       <c r="G4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H4" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I4" t="s">
         <v>76</v>
@@ -23197,7 +23201,7 @@
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A5" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>92</v>
@@ -23209,10 +23213,10 @@
         <v>400</v>
       </c>
       <c r="G5" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="H5" s="11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="I5" t="s">
         <v>76</v>
@@ -23310,7 +23314,7 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A6" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>92</v>
@@ -23322,10 +23326,10 @@
         <v>25</v>
       </c>
       <c r="G6" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H6" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I6" t="s">
         <v>77</v>
@@ -23334,7 +23338,7 @@
         <v>81</v>
       </c>
       <c r="K6" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M6" s="14">
         <v>0.26215664809918843</v>
@@ -23423,7 +23427,7 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A7" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>92</v>
@@ -23435,10 +23439,10 @@
         <v>50</v>
       </c>
       <c r="G7" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H7" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I7" t="s">
         <v>77</v>
@@ -23447,7 +23451,7 @@
         <v>81</v>
       </c>
       <c r="K7" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M7" s="14">
         <v>3.4539394319520054</v>
@@ -23536,7 +23540,7 @@
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A8" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>92</v>
@@ -23548,10 +23552,10 @@
         <v>75</v>
       </c>
       <c r="G8" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H8" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I8" t="s">
         <v>77</v>
@@ -23560,7 +23564,7 @@
         <v>81</v>
       </c>
       <c r="K8" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M8" s="14">
         <v>3.6536666666666666</v>
@@ -23649,7 +23653,7 @@
     </row>
     <row r="9" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>92</v>
@@ -23661,10 +23665,10 @@
         <v>100</v>
       </c>
       <c r="G9" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H9" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I9" t="s">
         <v>77</v>
@@ -23762,7 +23766,7 @@
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>92</v>
@@ -23774,10 +23778,10 @@
         <v>125</v>
       </c>
       <c r="G10" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H10" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I10" t="s">
         <v>77</v>
@@ -23875,7 +23879,7 @@
     </row>
     <row r="11" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A11" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>92</v>
@@ -23887,10 +23891,10 @@
         <v>150</v>
       </c>
       <c r="G11" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H11" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I11" t="s">
         <v>77</v>
@@ -23985,7 +23989,7 @@
     </row>
     <row r="12" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A12" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>92</v>
@@ -23997,10 +24001,10 @@
         <v>200</v>
       </c>
       <c r="G12" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H12" s="11" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="I12" t="s">
         <v>77</v>
@@ -24099,7 +24103,7 @@
     </row>
     <row r="13" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A13" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>92</v>
@@ -24111,10 +24115,10 @@
         <v>247.5</v>
       </c>
       <c r="G13" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H13" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I13" t="s">
         <v>77</v>
@@ -24212,7 +24216,7 @@
     </row>
     <row r="14" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A14" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>92</v>
@@ -24224,10 +24228,10 @@
         <v>402.5</v>
       </c>
       <c r="G14" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="H14" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I14" t="s">
         <v>77</v>
@@ -24325,7 +24329,7 @@
     </row>
     <row r="15" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>92</v>
@@ -24337,10 +24341,10 @@
         <v>600</v>
       </c>
       <c r="G15" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H15" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I15" t="s">
         <v>77</v>
@@ -24439,7 +24443,7 @@
     </row>
     <row r="16" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A16" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>92</v>
@@ -24451,10 +24455,10 @@
         <v>850</v>
       </c>
       <c r="G16" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H16" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I16" t="s">
         <v>77</v>
@@ -24553,7 +24557,7 @@
     </row>
     <row r="17" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>92</v>
@@ -24565,10 +24569,10 @@
         <v>1200</v>
       </c>
       <c r="G17" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="H17" s="11" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="I17" t="s">
         <v>77</v>
@@ -24667,7 +24671,7 @@
     </row>
     <row r="18" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A18" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>92</v>
@@ -24682,7 +24686,7 @@
         <v>5300</v>
       </c>
       <c r="H18" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I18" t="s">
         <v>75</v>
@@ -24691,7 +24695,7 @@
         <v>81</v>
       </c>
       <c r="K18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="M18" s="14">
         <v>3.1290724923146946</v>
@@ -24780,7 +24784,7 @@
     </row>
     <row r="19" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A19" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>92</v>
@@ -24795,7 +24799,7 @@
         <v>5300</v>
       </c>
       <c r="H19" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I19" t="s">
         <v>75</v>
@@ -24889,7 +24893,7 @@
     </row>
     <row r="20" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A20" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>92</v>
@@ -24904,7 +24908,7 @@
         <v>5300</v>
       </c>
       <c r="H20" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I20" t="s">
         <v>75</v>
@@ -25002,7 +25006,7 @@
     </row>
     <row r="21" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A21" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>92</v>
@@ -25017,7 +25021,7 @@
         <v>5300</v>
       </c>
       <c r="H21" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I21" t="s">
         <v>75</v>
@@ -25111,7 +25115,7 @@
     </row>
     <row r="22" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A22" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>92</v>
@@ -25126,7 +25130,7 @@
         <v>5300</v>
       </c>
       <c r="H22" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I22" t="s">
         <v>75</v>
@@ -25220,7 +25224,7 @@
     </row>
     <row r="23" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A23" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>92</v>
@@ -25235,7 +25239,7 @@
         <v>5300</v>
       </c>
       <c r="H23" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I23" t="s">
         <v>75</v>
@@ -25329,7 +25333,7 @@
     </row>
     <row r="24" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A24" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>92</v>
@@ -25344,7 +25348,7 @@
         <v>5300</v>
       </c>
       <c r="H24" s="11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="I24" t="s">
         <v>75</v>
@@ -25438,7 +25442,7 @@
     </row>
     <row r="25" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A25" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>92</v>
@@ -25457,6 +25461,9 @@
       </c>
       <c r="H25" s="20" t="s">
         <v>82</v>
+      </c>
+      <c r="I25" t="s">
+        <v>86</v>
       </c>
       <c r="J25" t="s">
         <v>80</v>
@@ -25535,7 +25542,7 @@
     </row>
     <row r="26" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A26" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>92</v>
@@ -25555,6 +25562,9 @@
       <c r="H26" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="I26" t="s">
+        <v>86</v>
+      </c>
       <c r="J26" t="s">
         <v>80</v>
       </c>
@@ -25648,7 +25658,7 @@
     </row>
     <row r="27" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A27" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>92</v>
@@ -25668,6 +25678,9 @@
       <c r="H27" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="I27" t="s">
+        <v>86</v>
+      </c>
       <c r="J27" t="s">
         <v>80</v>
       </c>
@@ -25761,7 +25774,7 @@
     </row>
     <row r="28" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A28" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>92</v>
@@ -25781,6 +25794,9 @@
       <c r="H28" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="I28" t="s">
+        <v>86</v>
+      </c>
       <c r="J28" t="s">
         <v>80</v>
       </c>
@@ -25874,7 +25890,7 @@
     </row>
     <row r="29" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>92</v>
@@ -25894,6 +25910,9 @@
       <c r="H29" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="I29" t="s">
+        <v>86</v>
+      </c>
       <c r="J29" t="s">
         <v>80</v>
       </c>
@@ -25987,7 +26006,7 @@
     </row>
     <row r="30" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A30" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>92</v>
@@ -26007,6 +26026,9 @@
       <c r="H30" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="I30" t="s">
+        <v>86</v>
+      </c>
       <c r="J30" t="s">
         <v>80</v>
       </c>
@@ -26100,7 +26122,7 @@
     </row>
     <row r="31" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A31" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>92</v>
@@ -26120,6 +26142,9 @@
       <c r="H31" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="I31" t="s">
+        <v>86</v>
+      </c>
       <c r="J31" t="s">
         <v>80</v>
       </c>
@@ -26213,7 +26238,7 @@
     </row>
     <row r="32" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A32" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>92</v>
@@ -26233,6 +26258,9 @@
       <c r="H32" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="I32" t="s">
+        <v>86</v>
+      </c>
       <c r="J32" t="s">
         <v>80</v>
       </c>
@@ -26326,7 +26354,7 @@
     </row>
     <row r="33" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A33" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>92</v>
@@ -26346,6 +26374,9 @@
       <c r="H33" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="I33" t="s">
+        <v>86</v>
+      </c>
       <c r="J33" t="s">
         <v>80</v>
       </c>
@@ -26439,7 +26470,7 @@
     </row>
     <row r="34" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A34" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>92</v>
@@ -26459,6 +26490,9 @@
       <c r="H34" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="I34" t="s">
+        <v>86</v>
+      </c>
       <c r="J34" t="s">
         <v>80</v>
       </c>
@@ -26552,7 +26586,7 @@
     </row>
     <row r="35" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A35" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>92</v>
@@ -26572,6 +26606,9 @@
       <c r="H35" s="21" t="s">
         <v>39</v>
       </c>
+      <c r="I35" t="s">
+        <v>86</v>
+      </c>
       <c r="J35" t="s">
         <v>80</v>
       </c>
@@ -26665,7 +26702,7 @@
     </row>
     <row r="36" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A36" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>92</v>
@@ -26685,6 +26722,9 @@
       <c r="H36" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="I36" t="s">
+        <v>86</v>
+      </c>
       <c r="J36" t="s">
         <v>80</v>
       </c>
@@ -26778,7 +26818,7 @@
     </row>
     <row r="37" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A37" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>92</v>
@@ -26798,6 +26838,9 @@
       <c r="H37" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="I37" t="s">
+        <v>86</v>
+      </c>
       <c r="J37" t="s">
         <v>80</v>
       </c>
@@ -26891,7 +26934,7 @@
     </row>
     <row r="38" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A38" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>92</v>
@@ -26911,6 +26954,9 @@
       <c r="H38" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="I38" t="s">
+        <v>86</v>
+      </c>
       <c r="J38" t="s">
         <v>80</v>
       </c>
@@ -27004,7 +27050,7 @@
     </row>
     <row r="39" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>92</v>
@@ -27024,6 +27070,9 @@
       <c r="H39" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="I39" t="s">
+        <v>86</v>
+      </c>
       <c r="J39" t="s">
         <v>80</v>
       </c>
@@ -27117,7 +27166,7 @@
     </row>
     <row r="40" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A40" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>92</v>
@@ -27137,6 +27186,9 @@
       <c r="H40" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="I40" t="s">
+        <v>86</v>
+      </c>
       <c r="J40" t="s">
         <v>80</v>
       </c>
@@ -27230,7 +27282,7 @@
     </row>
     <row r="41" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A41" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>92</v>
@@ -27250,6 +27302,9 @@
       <c r="H41" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="I41" t="s">
+        <v>86</v>
+      </c>
       <c r="J41" t="s">
         <v>80</v>
       </c>
@@ -27343,7 +27398,7 @@
     </row>
     <row r="42" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A42" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>92</v>
@@ -27363,6 +27418,9 @@
       <c r="H42" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="I42" t="s">
+        <v>86</v>
+      </c>
       <c r="J42" t="s">
         <v>80</v>
       </c>
@@ -27456,7 +27514,7 @@
     </row>
     <row r="43" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A43" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>92</v>
@@ -27476,6 +27534,9 @@
       <c r="H43" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="I43" t="s">
+        <v>86</v>
+      </c>
       <c r="J43" t="s">
         <v>80</v>
       </c>
@@ -27569,7 +27630,7 @@
     </row>
     <row r="44" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A44" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>92</v>
@@ -27589,6 +27650,9 @@
       <c r="H44" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="I44" t="s">
+        <v>86</v>
+      </c>
       <c r="J44" t="s">
         <v>80</v>
       </c>
@@ -27682,7 +27746,7 @@
     </row>
     <row r="45" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A45" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>92</v>
@@ -27702,6 +27766,9 @@
       <c r="H45" s="21" t="s">
         <v>41</v>
       </c>
+      <c r="I45" t="s">
+        <v>86</v>
+      </c>
       <c r="J45" t="s">
         <v>80</v>
       </c>
@@ -27795,7 +27862,7 @@
     </row>
     <row r="46" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A46" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>92</v>
@@ -27810,13 +27877,16 @@
         <v>25</v>
       </c>
       <c r="H46" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I46" t="s">
+        <v>87</v>
       </c>
       <c r="J46" t="s">
         <v>80</v>
       </c>
       <c r="K46" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="M46" s="24">
         <v>8.9056666666666668</v>
@@ -27901,7 +27971,7 @@
     </row>
     <row r="47" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A47" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>92</v>
@@ -27916,13 +27986,16 @@
         <v>400</v>
       </c>
       <c r="H47" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I47" t="s">
+        <v>87</v>
       </c>
       <c r="J47" t="s">
         <v>80</v>
       </c>
       <c r="K47" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="M47" s="24"/>
       <c r="N47" s="24">
@@ -27989,7 +28062,7 @@
     </row>
     <row r="48" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A48" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>92</v>
@@ -28004,13 +28077,16 @@
         <v>1250</v>
       </c>
       <c r="H48" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I48" t="s">
+        <v>87</v>
       </c>
       <c r="J48" t="s">
         <v>80</v>
       </c>
       <c r="K48" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="M48" s="24">
         <v>20.712499999999999</v>
@@ -28083,7 +28159,7 @@
     </row>
     <row r="49" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A49" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>92</v>
@@ -28098,13 +28174,16 @@
         <v>25</v>
       </c>
       <c r="H49" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I49" t="s">
+        <v>88</v>
       </c>
       <c r="J49" t="s">
         <v>80</v>
       </c>
       <c r="K49" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="M49" s="24">
         <v>12.197000000000001</v>
@@ -28189,7 +28268,7 @@
     </row>
     <row r="50" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A50" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>92</v>
@@ -28204,13 +28283,16 @@
         <v>400</v>
       </c>
       <c r="H50" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I50" t="s">
+        <v>88</v>
       </c>
       <c r="J50" t="s">
         <v>80</v>
       </c>
       <c r="K50" t="s">
-        <v>88</v>
+        <v>135</v>
       </c>
       <c r="M50" s="24">
         <v>24.502666666666666</v>
@@ -28299,7 +28381,7 @@
     </row>
     <row r="51" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A51" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>92</v>
@@ -28314,13 +28396,16 @@
         <v>400</v>
       </c>
       <c r="H51" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I51" t="s">
+        <v>91</v>
       </c>
       <c r="J51" t="s">
         <v>80</v>
       </c>
       <c r="K51" t="s">
-        <v>91</v>
+        <v>135</v>
       </c>
       <c r="M51" s="24">
         <v>12.996</v>
@@ -28405,7 +28490,7 @@
     </row>
     <row r="52" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A52" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>92</v>
@@ -28420,13 +28505,16 @@
         <v>25</v>
       </c>
       <c r="H52" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I52" t="s">
+        <v>103</v>
       </c>
       <c r="J52" t="s">
         <v>80</v>
       </c>
       <c r="K52" t="s">
-        <v>104</v>
+        <v>135</v>
       </c>
       <c r="M52" s="24">
         <v>16.220333333333333</v>
@@ -28511,7 +28599,7 @@
     </row>
     <row r="53" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A53" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>92</v>
@@ -28526,13 +28614,16 @@
         <v>25</v>
       </c>
       <c r="H53" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I53" t="s">
+        <v>89</v>
       </c>
       <c r="J53" t="s">
         <v>80</v>
       </c>
       <c r="K53" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="M53" s="24">
         <v>12.790666666666667</v>
@@ -28617,7 +28708,7 @@
     </row>
     <row r="54" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A54" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>92</v>
@@ -28632,13 +28723,16 @@
         <v>400</v>
       </c>
       <c r="H54" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I54" t="s">
+        <v>89</v>
       </c>
       <c r="J54" t="s">
         <v>80</v>
       </c>
       <c r="K54" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="M54" s="24">
         <v>16.561666666666667</v>
@@ -28723,7 +28817,7 @@
     </row>
     <row r="55" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A55" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>92</v>
@@ -28738,13 +28832,16 @@
         <v>1250</v>
       </c>
       <c r="H55" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I55" t="s">
+        <v>89</v>
       </c>
       <c r="J55" t="s">
         <v>80</v>
       </c>
       <c r="K55" t="s">
-        <v>89</v>
+        <v>135</v>
       </c>
       <c r="M55" s="24">
         <v>18.637</v>
@@ -28829,7 +28926,7 @@
     </row>
     <row r="56" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A56" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>92</v>
@@ -28844,13 +28941,16 @@
         <v>25</v>
       </c>
       <c r="H56" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I56" t="s">
+        <v>90</v>
       </c>
       <c r="J56" t="s">
         <v>80</v>
       </c>
       <c r="K56" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="M56" s="24">
         <v>16.039333333333332</v>
@@ -28935,7 +29035,7 @@
     </row>
     <row r="57" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A57" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>92</v>
@@ -28950,13 +29050,16 @@
         <v>400</v>
       </c>
       <c r="H57" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I57" t="s">
+        <v>90</v>
       </c>
       <c r="J57" t="s">
         <v>80</v>
       </c>
       <c r="K57" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="M57" s="24">
         <v>18.590333333333334</v>
@@ -29041,7 +29144,7 @@
     </row>
     <row r="58" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A58" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>92</v>
@@ -29056,13 +29159,16 @@
         <v>1250</v>
       </c>
       <c r="H58" s="22" t="s">
-        <v>94</v>
+        <v>135</v>
+      </c>
+      <c r="I58" t="s">
+        <v>90</v>
       </c>
       <c r="J58" t="s">
         <v>80</v>
       </c>
       <c r="K58" t="s">
-        <v>90</v>
+        <v>135</v>
       </c>
       <c r="M58" s="24">
         <v>24.252749999999999</v>
@@ -29147,7 +29253,7 @@
     </row>
     <row r="59" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A59" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B59" s="6" t="s">
         <v>92</v>
@@ -29155,11 +29261,14 @@
       <c r="F59">
         <v>7.5</v>
       </c>
-      <c r="H59" s="22" t="s">
-        <v>94</v>
+      <c r="H59" t="s">
+        <v>105</v>
+      </c>
+      <c r="I59" t="s">
+        <v>105</v>
       </c>
       <c r="J59" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K59" t="s">
         <v>85</v>
@@ -29233,7 +29342,7 @@
     </row>
     <row r="60" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A60" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B60" s="6" t="s">
         <v>92</v>
@@ -29241,11 +29350,14 @@
       <c r="F60">
         <v>7.5</v>
       </c>
-      <c r="H60" s="22" t="s">
-        <v>94</v>
+      <c r="H60" t="s">
+        <v>105</v>
+      </c>
+      <c r="I60" t="s">
+        <v>105</v>
       </c>
       <c r="J60" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K60" t="s">
         <v>85</v>
@@ -29319,7 +29431,7 @@
     </row>
     <row r="61" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A61" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B61" s="6" t="s">
         <v>92</v>
@@ -29327,11 +29439,14 @@
       <c r="F61">
         <v>400</v>
       </c>
-      <c r="H61" s="22" t="s">
-        <v>94</v>
+      <c r="H61" t="s">
+        <v>105</v>
+      </c>
+      <c r="I61" t="s">
+        <v>105</v>
       </c>
       <c r="J61" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K61" t="s">
         <v>85</v>
@@ -29405,7 +29520,7 @@
     </row>
     <row r="62" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A62" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B62" s="6" t="s">
         <v>92</v>
@@ -29413,11 +29528,14 @@
       <c r="F62">
         <v>850</v>
       </c>
-      <c r="H62" s="22" t="s">
-        <v>94</v>
+      <c r="H62" t="s">
+        <v>105</v>
+      </c>
+      <c r="I62" t="s">
+        <v>105</v>
       </c>
       <c r="J62" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K62" t="s">
         <v>85</v>
@@ -29494,7 +29612,7 @@
     </row>
     <row r="63" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A63" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B63" s="6" t="s">
         <v>92</v>
@@ -29502,11 +29620,14 @@
       <c r="F63">
         <v>2500</v>
       </c>
-      <c r="H63" s="22" t="s">
-        <v>94</v>
+      <c r="H63" t="s">
+        <v>105</v>
+      </c>
+      <c r="I63" t="s">
+        <v>105</v>
       </c>
       <c r="J63" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K63" t="s">
         <v>85</v>
@@ -29574,7 +29695,7 @@
     </row>
     <row r="64" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A64" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B64" s="6" t="s">
         <v>92</v>
@@ -29582,11 +29703,14 @@
       <c r="F64">
         <v>7.5</v>
       </c>
-      <c r="H64" s="22" t="s">
-        <v>94</v>
+      <c r="H64" t="s">
+        <v>105</v>
+      </c>
+      <c r="I64" t="s">
+        <v>105</v>
       </c>
       <c r="J64" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K64" t="s">
         <v>84</v>
@@ -29660,7 +29784,7 @@
     </row>
     <row r="65" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A65" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B65" s="6" t="s">
         <v>92</v>
@@ -29668,11 +29792,14 @@
       <c r="F65">
         <v>7.5</v>
       </c>
-      <c r="H65" s="22" t="s">
-        <v>94</v>
+      <c r="H65" t="s">
+        <v>105</v>
+      </c>
+      <c r="I65" t="s">
+        <v>105</v>
       </c>
       <c r="J65" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K65" t="s">
         <v>84</v>
@@ -29740,7 +29867,7 @@
     </row>
     <row r="66" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A66" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B66" s="6" t="s">
         <v>92</v>
@@ -29748,11 +29875,14 @@
       <c r="F66">
         <v>400</v>
       </c>
-      <c r="H66" s="22" t="s">
-        <v>94</v>
+      <c r="H66" t="s">
+        <v>105</v>
+      </c>
+      <c r="I66" t="s">
+        <v>105</v>
       </c>
       <c r="J66" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K66" t="s">
         <v>84</v>
@@ -29832,7 +29962,7 @@
     </row>
     <row r="67" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A67" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B67" s="6" t="s">
         <v>92</v>
@@ -29840,11 +29970,14 @@
       <c r="F67">
         <v>850</v>
       </c>
-      <c r="H67" s="22" t="s">
-        <v>94</v>
+      <c r="H67" t="s">
+        <v>105</v>
+      </c>
+      <c r="I67" t="s">
+        <v>105</v>
       </c>
       <c r="J67" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K67" t="s">
         <v>84</v>
@@ -29924,7 +30057,7 @@
     </row>
     <row r="68" spans="1:40" x14ac:dyDescent="0.75">
       <c r="A68" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B68" s="6" t="s">
         <v>92</v>
@@ -29932,11 +30065,14 @@
       <c r="F68">
         <v>2500</v>
       </c>
-      <c r="H68" s="22" t="s">
-        <v>94</v>
+      <c r="H68" t="s">
+        <v>105</v>
+      </c>
+      <c r="I68" t="s">
+        <v>105</v>
       </c>
       <c r="J68" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K68" t="s">
         <v>84</v>

</xml_diff>